<commit_message>
Ajout de nouvelles caractéristiques
</commit_message>
<xml_diff>
--- a/Data/fhr_stats.xlsx
+++ b/Data/fhr_stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Challenges\MathAData\FetalHeartRate\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155D389F-6ECC-4DDF-B0B9-3F76DF039A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B90B2B-46E6-49D9-B399-67742F6AD45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11520" activeTab="1" xr2:uid="{75A812B7-792C-4586-905A-35E92CF714BC}"/>
   </bookViews>
   <sheets>
     <sheet name="fhr_stats" sheetId="1" r:id="rId1"/>
-    <sheet name="Precision Moyenne" sheetId="5" r:id="rId2"/>
-    <sheet name="F1 Score" sheetId="4" r:id="rId3"/>
+    <sheet name="Précision Moyenne" sheetId="6" r:id="rId2"/>
+    <sheet name="Précision Moyenne (old)" sheetId="5" r:id="rId3"/>
     <sheet name="Moyennes" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="Volatilités" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
   <si>
     <t>ids</t>
   </si>
@@ -155,34 +155,17 @@
     <t>sujet sain si l'étendue de l'électrocardiogramme est inférieur à un seuil.</t>
   </si>
   <si>
-    <t>sujet sain si la moyenne de l'électrocardiogramme est inférieur à un seuil.</t>
-  </si>
-  <si>
-    <t>sujet sain si la volatilité de l'électrocardiogramme est inférieur à un seuil.</t>
-  </si>
-  <si>
     <t>Caractéristique</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>sujet sain si le % de points autour de la moyenne est supérieur à un seuil.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>sujet sain si le % de points dans un intervalle donné est inférieur à un seuil.
-(avec ajustement à la moyenne)</t>
   </si>
   <si>
     <t>sujet sain si le % de points dans un intervalle donné est supérieur à un seuil.
 (avec ajustement à la moyenne)</t>
-  </si>
-  <si>
-    <t>sujet sain si le % de points dans un intervalle donné est inférieur à un seuil.
-(sans ajustement à la moyenne)</t>
   </si>
   <si>
     <t>1A</t>
@@ -191,21 +174,8 @@
     <t>1B</t>
   </si>
   <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>sujet sain si le % de points au dessus de la moyenne de l'électrocardiogramme
-est inférieur à un seuil.</t>
-  </si>
-  <si>
     <t>sujet sain si le % de points dans l'intervalle [k1*moyenne, (1+k2)*moyenne]
 est supérieur à un seuil.</t>
-  </si>
-  <si>
-    <t>F1 Score</t>
   </si>
   <si>
     <t>sujet sain si le pourcentage de points dans l'intervalle [ 0, k]
@@ -214,14 +184,6 @@
   <si>
     <t>sujet sain si le pourcentage de points dans l'intervalle [ 0, k]
 est supérieurà un seuil.</t>
-  </si>
-  <si>
-    <t>5
-(moyenne)</t>
-  </si>
-  <si>
-    <t>7
-(volatilié)</t>
   </si>
   <si>
     <t>3
@@ -252,6 +214,175 @@
     <t>Nombre 
 d'hyperparamètres</t>
   </si>
+  <si>
+    <t>5A
+(moyenne)</t>
+  </si>
+  <si>
+    <t>5B
+(médiane)</t>
+  </si>
+  <si>
+    <t>sujet sain si la moyenne de l'électrocardiogramme
+est dans l'intervalle [k1, k2].</t>
+  </si>
+  <si>
+    <t>sujet sain si la médiane de l'électrocardiogramme
+est dans l'intervalle [k1, k2].</t>
+  </si>
+  <si>
+    <t>9i</t>
+  </si>
+  <si>
+    <t>1Ai</t>
+  </si>
+  <si>
+    <t>(complément de 1A)
+sujet sain si le % de points dans un intervalle donné est inférieur à un seuil.
+(avec ajustement à la moyenne)</t>
+  </si>
+  <si>
+    <t>sujet sain si le % de points dans un intervalle donné est supérieur à un seuil.
+(sans ajustement à la moyenne)</t>
+  </si>
+  <si>
+    <t>(complément de 1B)
+sujet sain si le % de points dans un intervalle donné est inférieur à un seuil.
+(sans ajustement à la moyenne)</t>
+  </si>
+  <si>
+    <t>1Bi</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>sujet sain si le pourcentage de fois où une valeur 'k' a été passée
+est &gt; à un seuil</t>
+  </si>
+  <si>
+    <t>14A</t>
+  </si>
+  <si>
+    <t>sujet sain si le pourcentage de passage par la moyenne
+est &gt; à un seuil.</t>
+  </si>
+  <si>
+    <t>14B</t>
+  </si>
+  <si>
+    <t>sujet sain si le pourcentage de passage par la médiane
+est &gt; à un seuil.</t>
+  </si>
+  <si>
+    <t>13i</t>
+  </si>
+  <si>
+    <t>(complément de 13)
+sujet sain si le pourcentage de fois où une valeur 'k' a été passée
+est &lt; à un seuil</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>sujet sain si le % de points autour de la médiane
+est supérieur à un seuil.</t>
+  </si>
+  <si>
+    <t>écart type autour de la médiane</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>sujet sain si la volatilité de l'électrocardiogramme
+est inférieur à un seuil.</t>
+  </si>
+  <si>
+    <t>sujet sain si le % de points autour de la moyenne
+est supérieur à un seuil.</t>
+  </si>
+  <si>
+    <t>sujet sain si l'écart type autour de la médiane
+est inférieur à un seuil.</t>
+  </si>
+  <si>
+    <t>sujet sain si le nombre de passage par la médiane
+(par unité de temps) est &gt; à un seuil.</t>
+  </si>
+  <si>
+    <t>sujet sain si le nombre de passage par la moyenne
+(par unité de temps) est &gt; à un seuil.</t>
+  </si>
+  <si>
+    <t>7A
+(volatilié)</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Précision Moyenne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(accuracy(label0)+accuracy(label1) / 2
+(sur toute la durée)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Précision Moyenne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(sur la dernière heure)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Précision Moyenne
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(sur la première heure)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -260,7 +391,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,8 +550,89 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,6 +818,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -753,66 +971,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -910,48 +1068,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -973,33 +1090,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1024,6 +1117,115 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1074,7 +1276,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1085,99 +1287,246 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="34" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1185,6 +1534,57 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -28752,7 +29152,7 @@
         <v>1</v>
       </c>
       <c r="X258">
-        <f t="shared" ref="X258:X321" si="9">IF(W258=B258,1,0)</f>
+        <f t="shared" ref="X258:X301" si="9">IF(W258=B258,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -32035,11 +32435,542 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DF795B-1D69-4ED2-8851-D60B7C7C04E1}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="92" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="104" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="110" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="83" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="94" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="105" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="43">
+        <v>1</v>
+      </c>
+      <c r="D5" s="109">
+        <v>0.71875</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="74">
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="G5" s="102">
+        <v>0.74580000000000002</v>
+      </c>
+      <c r="H5" s="100">
+        <v>0.74790000000000001</v>
+      </c>
+      <c r="I5" s="100">
+        <v>0.73329999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="106" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="88">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10" t="str">
+        <f>E5</f>
+        <v>x</v>
+      </c>
+      <c r="E6" s="90">
+        <v>0.7208</v>
+      </c>
+      <c r="F6" s="37">
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="G6" s="102">
+        <v>0.75</v>
+      </c>
+      <c r="H6" s="100">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="I6" s="100">
+        <v>0.73950000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="31">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
+        <f>F5</f>
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="E7" s="10">
+        <f>F6</f>
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="F7" s="89">
+        <v>0.71875</v>
+      </c>
+      <c r="G7" s="102" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="100">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="I7" s="100">
+        <v>0.75629999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="108" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="52">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10">
+        <f>G5</f>
+        <v>0.74580000000000002</v>
+      </c>
+      <c r="E8" s="10">
+        <f>G6</f>
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="10" t="str">
+        <f>G7</f>
+        <v>x</v>
+      </c>
+      <c r="G8" s="103">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="H8" s="100">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="I8" s="100">
+        <v>0.76039999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="97">
+        <v>2</v>
+      </c>
+      <c r="D9" s="98">
+        <f>H5</f>
+        <v>0.74790000000000001</v>
+      </c>
+      <c r="E9" s="98">
+        <f>H6</f>
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="F9" s="98">
+        <f>H7</f>
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="G9" s="98">
+        <f>H8</f>
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="H9" s="99">
+        <v>0.72707999999999995</v>
+      </c>
+      <c r="I9" s="100" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="95" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="96" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="101">
+        <v>2</v>
+      </c>
+      <c r="D10" s="98">
+        <f>I5</f>
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="E10" s="98">
+        <f>I6</f>
+        <v>0.73950000000000005</v>
+      </c>
+      <c r="F10" s="98">
+        <f>I7</f>
+        <v>0.75629999999999997</v>
+      </c>
+      <c r="G10" s="98">
+        <f>I8</f>
+        <v>0.76039999999999996</v>
+      </c>
+      <c r="H10" s="98" t="str">
+        <f>I9</f>
+        <v>x</v>
+      </c>
+      <c r="I10" s="99">
+        <v>0.72707999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="32.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="93"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="32.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="93"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="83" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="43">
+        <v>1</v>
+      </c>
+      <c r="D19" s="89">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="74">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="G19" s="84">
+        <v>0.77290000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="88">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10" t="str">
+        <f>E19</f>
+        <v>x</v>
+      </c>
+      <c r="E20" s="90">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F20" s="37">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="G20" s="84">
+        <v>0.76670000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="31">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10">
+        <f>F19</f>
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="E21" s="10">
+        <f>F20</f>
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F21" s="89">
+        <v>0.70409999999999995</v>
+      </c>
+      <c r="G21" s="84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="52">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10">
+        <f>G19</f>
+        <v>0.77290000000000003</v>
+      </c>
+      <c r="E22" s="10">
+        <f>G20</f>
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F22" s="10" t="str">
+        <f>G21</f>
+        <v>x</v>
+      </c>
+      <c r="G22" s="91">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:7" ht="32.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="93"/>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="32.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="93"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:7" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="83" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="43">
+        <v>1</v>
+      </c>
+      <c r="D28" s="89">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="E28" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="74">
+        <v>0.77290000000000003</v>
+      </c>
+      <c r="G28" s="84">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="85" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="88">
+        <v>1</v>
+      </c>
+      <c r="D29" s="10" t="str">
+        <f>E28</f>
+        <v>x</v>
+      </c>
+      <c r="E29" s="90">
+        <v>0.77290000000000003</v>
+      </c>
+      <c r="F29" s="37">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="G29" s="84">
+        <v>0.77910000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="31">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10">
+        <f>F28</f>
+        <v>0.77290000000000003</v>
+      </c>
+      <c r="E30" s="10">
+        <f>F29</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F30" s="89">
+        <v>0.62909999999999999</v>
+      </c>
+      <c r="G30" s="84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="52">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10">
+        <f>G28</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E31" s="10">
+        <f>G29</f>
+        <v>0.77910000000000001</v>
+      </c>
+      <c r="F31" s="10" t="str">
+        <f>G30</f>
+        <v>x</v>
+      </c>
+      <c r="G31" s="91">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A15:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63C614A-7386-43A6-9DD4-2AB06226689D}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32047,1192 +32978,1048 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="17"/>
+    <col min="6" max="6" width="9.140625" style="17"/>
+    <col min="11" max="11" width="9.140625" style="17"/>
+    <col min="12" max="12" width="9.140625" style="47"/>
+    <col min="14" max="15" width="9.140625" style="17"/>
+    <col min="19" max="19" width="9.140625" style="47"/>
+    <col min="20" max="20" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="26"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+    <row r="1" spans="1:22" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="92" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:22" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="23">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="75">
+        <v>6</v>
+      </c>
+      <c r="L4" s="11">
+        <v>7</v>
+      </c>
+      <c r="M4" s="41">
+        <v>8</v>
+      </c>
+      <c r="N4" s="23">
+        <v>9</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>13</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="80">
+        <v>3</v>
+      </c>
+      <c r="D5" s="77">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="F5" s="19">
+        <v>0.77290999999999999</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0.74170000000000003</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0.71660000000000001</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="L5" s="46">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="M5" s="19">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="N5" s="19">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="O5" s="19">
+        <v>0.74170000000000003</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="46">
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="T5" s="36">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+    </row>
+    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="21">
         <v>3</v>
       </c>
-      <c r="I4" s="7">
-        <v>4</v>
-      </c>
-      <c r="J4" s="8">
-        <v>5</v>
-      </c>
-      <c r="K4" s="15">
-        <v>6</v>
-      </c>
-      <c r="L4" s="15">
-        <v>7</v>
-      </c>
-      <c r="M4" s="27">
-        <v>8</v>
-      </c>
-      <c r="N4" s="7">
-        <v>9</v>
-      </c>
-      <c r="O4" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="35">
-        <v>3</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.73329999999999995</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="11">
-        <v>0.77290999999999999</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0.74170000000000003</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0.71660000000000001</v>
-      </c>
-      <c r="I5" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0.73540000000000005</v>
-      </c>
-      <c r="K5" s="11">
-        <v>0.73540000000000005</v>
-      </c>
-      <c r="L5" s="11">
-        <v>0.73750000000000004</v>
-      </c>
-      <c r="M5" s="11">
-        <v>0.73329999999999995</v>
-      </c>
-      <c r="N5" s="11">
-        <v>0.73540000000000005</v>
-      </c>
-      <c r="O5" s="11">
-        <v>0.74170000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="36">
-        <v>3</v>
-      </c>
-      <c r="D6" s="12" t="str">
+      <c r="D6" s="16" t="str">
         <f>E5</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="18">
         <v>0.70625000000000004</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="19">
         <v>0.74170000000000003</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="19">
         <v>0.71040000000000003</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="19">
         <v>0.71450000000000002</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="19">
         <v>0.72909999999999997</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="19">
         <v>0.70409999999999995</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="19">
         <v>0.69579999999999997</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="46">
         <v>0.73329999999999995</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="19">
         <v>0.71240000000000003</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="19">
         <v>0.70625000000000004</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="19">
         <v>0.69579999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="36">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="46">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="T6" s="58">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" s="69" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="65">
         <v>3</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="61">
         <f>F5</f>
         <v>0.77290999999999999</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="61">
         <f>F6</f>
         <v>0.74170000000000003</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="66">
         <v>0.70416000000000001</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="11">
+      <c r="G7" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="62">
         <v>0.70208000000000004</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="62">
         <v>0.76449999999999996</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="62">
         <v>0.71875</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="62">
         <v>0.71250000000000002</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="67">
         <v>0.75829999999999997</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="62">
         <v>0.74170000000000003</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="62">
         <v>0.72289999999999999</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="62">
         <v>0.72909999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="36">
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="67">
+        <v>0.74160000000000004</v>
+      </c>
+      <c r="T7" s="68">
+        <v>0.7208</v>
+      </c>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62">
+        <v>0.73540000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="21">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="16">
         <f>G5</f>
         <v>0.74170000000000003</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="16">
         <f>G6</f>
         <v>0.71040000000000003</v>
       </c>
-      <c r="F8" s="12" t="str">
+      <c r="F8" s="16" t="str">
         <f>G7</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G8" s="9">
-        <v>0.6895</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="G8" s="18">
+        <v>0.69579999999999997</v>
+      </c>
+      <c r="H8" s="19">
         <v>0.69159999999999999</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="19">
         <v>0.74370000000000003</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="19">
         <v>0.67910000000000004</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="19">
         <v>7.0400000000000003E-3</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="46">
         <v>0.72291000000000005</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="19">
         <v>0.71250000000000002</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="19">
         <v>0.70830000000000004</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="19">
         <v>0.69579999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="29" t="s">
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="46">
+        <v>0.72289999999999999</v>
+      </c>
+      <c r="T8" s="58">
+        <v>0.7</v>
+      </c>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="37">
-        <v>2</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="C9" s="15">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
         <f>H5</f>
         <v>0.71660000000000001</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="16">
         <f>H6</f>
         <v>0.71450000000000002</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="16">
         <f>H7</f>
         <v>0.70208000000000004</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="16">
         <f>H8</f>
         <v>0.69159999999999999</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="18">
         <v>0.60199999999999998</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="19">
         <v>0.73540000000000005</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="19">
         <v>0.64159999999999995</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="19">
         <v>0.6583</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="46">
         <v>0.71875</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="19">
         <v>0.71199999999999997</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="19">
         <v>0.68330000000000002</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="19">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
-        <v>4</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="37">
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="46">
+        <v>0.69588000000000005</v>
+      </c>
+      <c r="T9" s="58">
+        <v>0.65625</v>
+      </c>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="1:22" s="47" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="44">
         <v>2</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="45">
         <f>I5</f>
         <v>0.75</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="45">
         <f>I6</f>
         <v>0.72909999999999997</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="45">
         <f>I7</f>
         <v>0.76449999999999996</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="45">
         <f>I8</f>
         <v>0.74370000000000003</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="45">
         <f>I9</f>
         <v>0.73540000000000005</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>0.72707999999999995</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="11">
+      <c r="J10" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="37">
         <v>0.74790000000000001</v>
       </c>
-      <c r="M10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="37">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="M10" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="37">
+        <v>0.75409999999999999</v>
+      </c>
+      <c r="T10" s="59">
+        <v>0.76039999999999996</v>
+      </c>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+    </row>
+    <row r="11" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="15">
+        <v>2</v>
+      </c>
+      <c r="D11" s="16">
         <f>J5</f>
         <v>0.73540000000000005</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="16">
         <f>J6</f>
         <v>0.70409999999999995</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="16">
         <f>J7</f>
         <v>0.71875</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="16">
         <f>J8</f>
         <v>0.67910000000000004</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="16">
         <f>J9</f>
         <v>0.64159999999999995</v>
       </c>
-      <c r="I11" s="12" t="str">
+      <c r="I11" s="16" t="str">
         <f>J10</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="18">
         <v>0.57909999999999995</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="11">
+      <c r="K11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="46">
         <v>0.7208</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="M11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="46">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="T11" s="58">
+        <v>0.66869999999999996</v>
+      </c>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:22" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
         <v>6</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="36">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12">
+      <c r="B12" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
         <f>K5</f>
         <v>0.73540000000000005</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="16">
         <f>K6</f>
         <v>0.69579999999999997</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="16">
         <f>K7</f>
         <v>0.71250000000000002</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="16">
         <f>K8</f>
         <v>7.0400000000000003E-3</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="16">
         <f>K9</f>
         <v>0.6583</v>
       </c>
-      <c r="I12" s="12" t="str">
+      <c r="I12" s="16" t="str">
         <f>K10</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J12" s="12" t="str">
+      <c r="J12" s="16" t="str">
         <f>K11</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="38">
         <v>0.629</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="46">
         <v>0.73299999999999998</v>
       </c>
-      <c r="M12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="37">
-        <v>1</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="M12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+    </row>
+    <row r="13" spans="1:22" s="54" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="71">
+        <v>1</v>
+      </c>
+      <c r="D13" s="45">
         <f>L5</f>
         <v>0.73750000000000004</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="72">
         <f>L6</f>
         <v>0.73329999999999995</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="72">
         <f>L7</f>
         <v>0.75829999999999997</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="72">
         <f>L8</f>
         <v>0.72291000000000005</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="72">
         <f>L9</f>
         <v>0.71875</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="72">
         <f>L10</f>
         <v>0.74790000000000001</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="72">
         <f>L11</f>
         <v>0.7208</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="45">
         <f>L12</f>
         <v>0.73299999999999998</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="73">
         <v>0.71875</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="74">
         <v>0.72499999999999998</v>
       </c>
-      <c r="N13" s="11">
-        <v>0.71875</v>
-      </c>
-      <c r="O13" s="11">
+      <c r="N13" s="46">
+        <v>0.7208</v>
+      </c>
+      <c r="O13" s="46">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74">
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="T13" s="59">
+        <v>0.74580000000000002</v>
+      </c>
+      <c r="U13" s="74">
         <v>0.73329999999999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="V13" s="74"/>
+    </row>
+    <row r="14" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
         <v>8</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="36">
+      <c r="B14" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="21">
         <v>3</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="16">
         <f>M5</f>
         <v>0.73329999999999995</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="16">
         <f>M6</f>
         <v>0.71240000000000003</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="16">
         <f>M7</f>
         <v>0.74170000000000003</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="16">
         <f>M8</f>
         <v>0.71250000000000002</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="16">
         <f>M9</f>
         <v>0.71199999999999997</v>
       </c>
-      <c r="I14" s="12" t="str">
+      <c r="I14" s="16" t="str">
         <f>M10</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J14" s="12" t="str">
+      <c r="J14" s="16" t="str">
         <f>M11</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="K14" s="12" t="str">
+      <c r="K14" s="16" t="str">
         <f>M12</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="45">
         <f>M13</f>
         <v>0.72499999999999998</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="38">
         <v>0.71450000000000002</v>
       </c>
-      <c r="N14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="N14" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="O14" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="46">
+        <v>0.74790000000000001</v>
+      </c>
+      <c r="T14" s="58">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+    </row>
+    <row r="15" spans="1:22" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <v>9</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="36">
+      <c r="B15" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="21">
         <v>2</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="16">
         <f>N5</f>
         <v>0.73540000000000005</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="16">
         <f>N6</f>
         <v>0.70625000000000004</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="16">
         <f>N7</f>
         <v>0.72289999999999999</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="16">
         <f>N8</f>
         <v>0.70830000000000004</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="16">
         <f>N9</f>
         <v>0.68330000000000002</v>
       </c>
-      <c r="I15" s="12" t="str">
+      <c r="I15" s="16" t="str">
         <f>N10</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J15" s="12" t="str">
+      <c r="J15" s="16" t="str">
         <f>N11</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="K15" s="12" t="str">
+      <c r="K15" s="16" t="str">
         <f>N12</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="45">
         <f>N13</f>
-        <v>0.71875</v>
-      </c>
-      <c r="M15" s="12" t="str">
+        <v>0.7208</v>
+      </c>
+      <c r="M15" s="16" t="str">
         <f>N14</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="38">
         <v>0.67910000000000004</v>
       </c>
-      <c r="O15" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
-        <v>10</v>
-      </c>
-      <c r="B16" s="28" t="s">
+      <c r="O15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="46">
+        <v>0.72709999999999997</v>
+      </c>
+      <c r="T15" s="36">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="U15" s="19">
+        <v>0.74370000000000003</v>
+      </c>
+      <c r="V15" s="19"/>
+    </row>
+    <row r="16" spans="1:22" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="36">
+      <c r="B16" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="21">
         <v>2</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="16">
         <f>O5</f>
         <v>0.74170000000000003</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="16">
         <f>O6</f>
         <v>0.69579999999999997</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="16">
         <f>O7</f>
         <v>0.72909999999999997</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="16">
         <f>O8</f>
         <v>0.69579999999999997</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="16">
         <f>O9</f>
         <v>0.65</v>
       </c>
-      <c r="I16" s="12" t="str">
+      <c r="I16" s="16" t="str">
         <f>O10</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J16" s="12" t="str">
+      <c r="J16" s="16" t="str">
         <f>O11</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="K16" s="12" t="str">
+      <c r="K16" s="16" t="str">
         <f>O12</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="45">
         <f>O13</f>
-        <v>0.73329999999999995</v>
-      </c>
-      <c r="M16" s="12" t="str">
+        <v>0.73540000000000005</v>
+      </c>
+      <c r="M16" s="16" t="str">
         <f>O14</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="N16" s="12" t="str">
+      <c r="N16" s="16" t="str">
         <f>O15</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="18">
         <v>0.62080000000000002</v>
       </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25034967-0087-45F4-9CE5-3D7D9D1E0A8D}">
-  <dimension ref="A1:L14"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="40"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="7">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7">
-        <v>4</v>
-      </c>
-      <c r="I4" s="8">
-        <v>5</v>
-      </c>
-      <c r="J4" s="15">
-        <v>6</v>
-      </c>
-      <c r="K4" s="15">
-        <v>7</v>
-      </c>
-      <c r="L4" s="15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.76919999999999999</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="11">
-        <v>0.82509999999999994</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="12" t="str">
-        <f>D5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.63060000000000005</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="11">
-        <v>0.83540000000000003</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="12" t="str">
-        <f>E5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D7" s="12" t="str">
-        <f>E6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E7" s="9">
-        <v>0.68630000000000002</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="11">
-        <v>0.82</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="12" t="str">
-        <f>F5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D8" s="12" t="str">
-        <f>F6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E8" s="12" t="str">
-        <f>F7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.65449999999999997</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="11">
-        <v>0.78039999999999998</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
-        <v>3</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="12" t="str">
-        <f>G5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D9" s="12" t="str">
-        <f>G6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E9" s="12" t="str">
-        <f>G7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F9" s="12" t="str">
-        <f>G8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G9" s="9">
-        <v>0.47389999999999999</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="11">
-        <v>0.77110000000000001</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24">
-        <v>4</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="12" t="str">
-        <f>H5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D10" s="12" t="str">
-        <f>H6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E10" s="12" t="str">
-        <f>H7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F10" s="12" t="str">
-        <f>H8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G10" s="12" t="str">
-        <f>H9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H10" s="9">
-        <v>0.76539999999999997</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="11">
-        <v>0.8095</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
-        <v>5</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="12" t="str">
-        <f>I5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D11" s="12" t="str">
-        <f>I6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E11" s="12" t="str">
-        <f>I7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F11" s="12" t="str">
-        <f>I8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G11" s="12" t="str">
-        <f>I9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H11" s="12" t="str">
-        <f>I10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I11" s="9">
-        <v>0.45269999999999999</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
-        <v>6</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="12" t="str">
-        <f>J5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D12" s="12" t="str">
-        <f>J6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E12" s="12" t="str">
-        <f>J7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F12" s="12" t="str">
-        <f>J8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G12" s="12" t="str">
-        <f>J9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H12" s="12" t="str">
-        <f>J10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I12" s="12" t="str">
-        <f>J11</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="J12" s="18">
-        <v>0.50980000000000003</v>
-      </c>
-      <c r="K12" s="11">
-        <v>0.77410000000000001</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
-        <v>7</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="12">
-        <f>K5</f>
-        <v>0.82509999999999994</v>
-      </c>
-      <c r="D13" s="12">
-        <f>K6</f>
-        <v>0.83540000000000003</v>
-      </c>
-      <c r="E13" s="12">
-        <f>K7</f>
-        <v>0.82</v>
-      </c>
-      <c r="F13" s="12">
-        <f>K8</f>
-        <v>0.78039999999999998</v>
-      </c>
-      <c r="G13" s="12">
-        <f>K9</f>
-        <v>0.77110000000000001</v>
-      </c>
-      <c r="H13" s="12">
-        <f>K10</f>
-        <v>0.8095</v>
-      </c>
-      <c r="I13" s="12">
-        <f>K11</f>
-        <v>0.8</v>
-      </c>
-      <c r="J13" s="12">
-        <f>K12</f>
-        <v>0.77410000000000001</v>
-      </c>
-      <c r="K13" s="18">
-        <v>0.77110000000000001</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
-        <v>8</v>
-      </c>
-      <c r="B14" s="22" t="s">
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="46">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="T16" s="36"/>
+      <c r="U16" s="19">
+        <v>0.74170000000000003</v>
+      </c>
+      <c r="V16" s="19"/>
+    </row>
+    <row r="17" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="12" t="str">
-        <f>L5</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D14" s="12" t="str">
-        <f>L6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E14" s="12" t="str">
-        <f>L7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F14" s="12" t="str">
-        <f>L8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G14" s="12" t="str">
-        <f>L9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H14" s="12" t="str">
-        <f>L10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I14" s="12" t="str">
-        <f>L11</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="J14" s="12" t="str">
-        <f>L12</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K14" s="12" t="str">
-        <f>L13</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="L14" s="9">
-        <v>0.73119999999999996</v>
+      <c r="B17" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="17"/>
+      <c r="P17" s="18">
+        <v>0.57289999999999996</v>
+      </c>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="46">
+        <v>0.7</v>
+      </c>
+      <c r="T17" s="58">
+        <v>0.65210000000000001</v>
+      </c>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+    </row>
+    <row r="18" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>13</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="21">
+        <v>2</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="22">
+        <v>0.58540000000000003</v>
+      </c>
+      <c r="R18" s="19"/>
+      <c r="S18" s="46">
+        <v>0.71040000000000003</v>
+      </c>
+      <c r="T18" s="58"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="21">
+        <v>2</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="22">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="S19" s="46">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="T19" s="58">
+        <v>0.71040000000000003</v>
+      </c>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="50">
+        <v>1</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="73">
+        <v>0.71875</v>
+      </c>
+      <c r="T20" s="59">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="U20" s="37">
+        <v>0.75629999999999997</v>
+      </c>
+      <c r="V20" s="37">
+        <v>0.75829999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="53" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="51">
+        <v>1</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="54"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="55">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="51">
+        <v>2</v>
+      </c>
+      <c r="M22" s="17"/>
+      <c r="U22" s="8">
+        <v>0.72707999999999995</v>
+      </c>
+      <c r="V22" s="14">
+        <v>0.73960000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="51">
+        <v>1</v>
+      </c>
+      <c r="V23" s="14">
+        <v>0.7208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>